<commit_message>
Added Working Code with Connections Closed
</commit_message>
<xml_diff>
--- a/data/Name_Details.xlsx
+++ b/data/Name_Details.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giridharrajkumar/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giridharrajkumar/eclipse-workspace/FilloExample/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE1C94B5-1882-674D-8155-523276C3097F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561EFB3C-0C97-C84B-92FF-D97892F55617}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{49581A89-C0C5-2748-A03C-CD30D4CD6BEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -54,7 +54,16 @@
     <t>Ramprasad</t>
   </si>
   <si>
-    <t>Peter</t>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Mickey</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -407,15 +416,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16398C70-591A-BA47-B1A9-382EA059FEED}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,36 +437,43 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>35.0</v>
+      <c r="C2">
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>30</v>
+      <c r="C3" t="n">
+        <v>20.0</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -470,6 +486,63 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
+      <c r="E4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6"/>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6"/>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7"/>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>